<commit_message>
small fix create sujet
</commit_message>
<xml_diff>
--- a/uploads/students/students.xlsx
+++ b/uploads/students/students.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t xml:space="preserve">la9ab</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t xml:space="preserve">mami</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mokhtar</t>
   </si>
   <si>
     <t xml:space="preserve">mamimokhtar@gmail.com</t>
@@ -223,10 +226,10 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.06"/>
@@ -271,7 +274,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>1</v>
+        <v>1700203</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -291,7 +294,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>2</v>
+        <v>1700204</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -299,10 +302,10 @@
         <v>14</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>9</v>
@@ -311,7 +314,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>3</v>
+        <v>1700205</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>